<commit_message>
Redefine definition of financial cost as effective cost/loan ratio
Former-commit-id: 6ca64d61c64e073a31eb2db5a471af41f2c3e9a6
</commit_message>
<xml_diff>
--- a/Tables/oc_reg.xlsx
+++ b/Tables/oc_reg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2666F166-ECBC-41A5-B310-1F12F6A43D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26555E5-B7C7-4BAD-9CD9-DBA745C8B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D31716B-EE2F-4621-AE96-1D753AE0E1B5}"/>
+    <workbookView xWindow="-28920" yWindow="-6825" windowWidth="29040" windowHeight="15840" xr2:uid="{3D31716B-EE2F-4621-AE96-1D753AE0E1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="oc_reg" sheetId="2" r:id="rId1"/>
@@ -209,22 +209,22 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>0.0030</v>
+            <v>0.039</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-0.12</v>
+            <v>-0.16</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-0.043</v>
+            <v>0.010</v>
           </cell>
           <cell r="E5" t="str">
             <v>-0.16</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-10.7</v>
+            <v>-129.5</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-14.2</v>
+            <v>-125.0</v>
           </cell>
         </row>
         <row r="6">
@@ -235,7 +235,7 @@
             <v>(0.094)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(0.067)</v>
+            <v>(0.072)</v>
           </cell>
           <cell r="D6" t="str">
             <v>(0.14)</v>
@@ -244,30 +244,30 @@
             <v>(0.084)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(8.31)</v>
+            <v>(33.3)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(8.32)</v>
+            <v>(34.6)</v>
           </cell>
         </row>
         <row r="83">
           <cell r="B83" t="str">
-            <v>0.55</v>
+            <v>0.61</v>
           </cell>
           <cell r="C83" t="str">
-            <v>0.23</v>
+            <v>0.27</v>
           </cell>
           <cell r="D83" t="str">
-            <v>0.54</v>
+            <v>0.49</v>
           </cell>
           <cell r="E83" t="str">
-            <v>0.29</v>
+            <v>0.24</v>
           </cell>
           <cell r="F83" t="str">
-            <v>-137.6</v>
+            <v>-307.2</v>
           </cell>
           <cell r="G83" t="str">
-            <v>-154.9</v>
+            <v>-289.3</v>
           </cell>
         </row>
         <row r="84">
@@ -275,27 +275,27 @@
             <v>(0.12)</v>
           </cell>
           <cell r="C84" t="str">
-            <v>(0.081)</v>
+            <v>(0.086)</v>
           </cell>
           <cell r="D84" t="str">
-            <v>(0.17)</v>
+            <v>(0.18)</v>
           </cell>
           <cell r="E84" t="str">
             <v>(0.13)</v>
           </cell>
           <cell r="F84" t="str">
-            <v>(12.1)</v>
+            <v>(62.8)</v>
           </cell>
           <cell r="G84" t="str">
-            <v>(13.4)</v>
+            <v>(64.3)</v>
           </cell>
         </row>
         <row r="86">
           <cell r="B86" t="str">
-            <v>840</v>
+            <v>845</v>
           </cell>
           <cell r="C86" t="str">
-            <v>1029</v>
+            <v>1040</v>
           </cell>
           <cell r="D86" t="str">
             <v>678</v>
@@ -304,10 +304,10 @@
             <v>781</v>
           </cell>
           <cell r="F86" t="str">
-            <v>1266</v>
+            <v>1265</v>
           </cell>
           <cell r="G86" t="str">
-            <v>1266</v>
+            <v>1265</v>
           </cell>
         </row>
         <row r="87">
@@ -315,10 +315,10 @@
             <v>R-sq</v>
           </cell>
           <cell r="B87" t="str">
-            <v>0.190</v>
+            <v>0.189</v>
           </cell>
           <cell r="C87" t="str">
-            <v>0.138</v>
+            <v>0.137</v>
           </cell>
           <cell r="D87" t="str">
             <v>0.225</v>
@@ -327,10 +327,10 @@
             <v>0.162</v>
           </cell>
           <cell r="F87" t="str">
-            <v>0.123</v>
+            <v>0.042</v>
           </cell>
           <cell r="G87" t="str">
-            <v>0.129</v>
+            <v>0.043</v>
           </cell>
         </row>
         <row r="88">
@@ -350,7 +350,7 @@
             <v>0.15</v>
           </cell>
           <cell r="F88" t="str">
-            <v>-116.3</v>
+            <v>-323.2</v>
           </cell>
         </row>
       </sheetData>
@@ -728,7 +728,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>[1]oc_reg!C5</f>
-        <v>-0.12</v>
+        <v>-0.16</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>[1]oc_reg!E5</f>
@@ -736,19 +736,19 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>[1]oc_reg!B5</f>
-        <v>0.0030</v>
+        <v>0.039</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>[1]oc_reg!D5</f>
-        <v>-0.043</v>
+        <v>0.010</v>
       </c>
       <c r="F5" s="1" t="str">
         <f>[1]oc_reg!F5</f>
-        <v>-10.7</v>
+        <v>-129.5</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>[1]oc_reg!G5</f>
-        <v>-14.2</v>
+        <v>-125.0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -758,7 +758,7 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>[1]oc_reg!C6</f>
-        <v>(0.067)</v>
+        <v>(0.072)</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]oc_reg!E6</f>
@@ -774,11 +774,11 @@
       </c>
       <c r="F6" s="1" t="str">
         <f>[1]oc_reg!F6</f>
-        <v>(8.31)</v>
+        <v>(33.3)</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>[1]oc_reg!G6</f>
-        <v>(8.32)</v>
+        <v>(34.6)</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,33 +787,33 @@
       </c>
       <c r="B7" s="1" t="str">
         <f>[1]oc_reg!C83</f>
-        <v>0.23</v>
+        <v>0.27</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]oc_reg!E83</f>
-        <v>0.29</v>
+        <v>0.24</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>[1]oc_reg!B83</f>
-        <v>0.55</v>
+        <v>0.61</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>[1]oc_reg!D83</f>
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>[1]oc_reg!F83</f>
-        <v>-137.6</v>
+        <v>-307.2</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>[1]oc_reg!G83</f>
-        <v>-154.9</v>
+        <v>-289.3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="str">
         <f>[1]oc_reg!C84</f>
-        <v>(0.081)</v>
+        <v>(0.086)</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>[1]oc_reg!E84</f>
@@ -825,15 +825,15 @@
       </c>
       <c r="E8" s="1" t="str">
         <f>[1]oc_reg!D84</f>
-        <v>(0.17)</v>
+        <v>(0.18)</v>
       </c>
       <c r="F8" s="1" t="str">
         <f>[1]oc_reg!F84</f>
-        <v>(12.1)</v>
+        <v>(62.8)</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>[1]oc_reg!G84</f>
-        <v>(13.4)</v>
+        <v>(64.3)</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -850,7 +850,7 @@
       </c>
       <c r="B10" s="7" t="str">
         <f>[1]oc_reg!C86</f>
-        <v>1029</v>
+        <v>1040</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>[1]oc_reg!E86</f>
@@ -858,7 +858,7 @@
       </c>
       <c r="D10" s="7" t="str">
         <f>[1]oc_reg!B86</f>
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="E10" s="7" t="str">
         <f>[1]oc_reg!D86</f>
@@ -866,11 +866,11 @@
       </c>
       <c r="F10" s="7" t="str">
         <f>[1]oc_reg!F86</f>
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="G10" s="7" t="str">
         <f>[1]oc_reg!G86</f>
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -880,7 +880,7 @@
       </c>
       <c r="B11" s="1" t="str">
         <f>[1]oc_reg!C87</f>
-        <v>0.138</v>
+        <v>0.137</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>[1]oc_reg!E87</f>
@@ -888,7 +888,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f>[1]oc_reg!B87</f>
-        <v>0.190</v>
+        <v>0.189</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>[1]oc_reg!D87</f>
@@ -896,11 +896,11 @@
       </c>
       <c r="F11" s="1" t="str">
         <f>[1]oc_reg!F87</f>
-        <v>0.123</v>
+        <v>0.042</v>
       </c>
       <c r="G11" s="1" t="str">
         <f>[1]oc_reg!G87</f>
-        <v>0.129</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -926,7 +926,7 @@
       </c>
       <c r="F12" s="10" t="str">
         <f>[1]oc_reg!F88</f>
-        <v>-116.3</v>
+        <v>-323.2</v>
       </c>
       <c r="G12" s="10"/>
     </row>

</xml_diff>